<commit_message>
retrait de express et ajout de nextjs
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6566D8E5-36E1-A742-89A0-BDE93B4AAA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4FD86F-F50D-624E-99F4-CC9E08047524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -140,109 +140,55 @@
     <t>Exercice</t>
   </si>
   <si>
-    <t>Évaluation formative</t>
-  </si>
-  <si>
-    <t>Projet API</t>
-  </si>
-  <si>
-    <t>Examen API</t>
-  </si>
-  <si>
-    <t>Examen React</t>
-  </si>
-  <si>
-    <t>Projet Application React</t>
-  </si>
-  <si>
-    <t>[Exercice 1 - Node](exercice1_node.md)</t>
-  </si>
-  <si>
-    <t>[Introduction à Node.js](introduction_nodejs.md) &lt;br/&gt; [Introduction à TypeScript](introduction_typescript.md) &lt;br/&gt; [Node.js - Serveur Web](nodejs_serveur_web.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 2 - lodash](exercice2_lodash.md)</t>
-  </si>
-  <si>
-    <t>[npm](npm.md)</t>
-  </si>
-  <si>
-    <t>[TypeScript 2](typescript_2.md)&lt;br/&gt;[Introduction Express](introduction_express.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 3 - Express](exercice3_express.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 4 - Express avec modèle](exercice4_express_avec_modele.md)</t>
-  </si>
-  <si>
-    <t>[Express - Générateur](generateur_express.md)</t>
-  </si>
-  <si>
-    <t>[JavaScript asynchrone](javascript_async.md) &lt;br/&gt; [MongoDB](mongodb.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 5 - MongoDB](exercice5_mongodb.md)</t>
-  </si>
-  <si>
-    <t>[Mongoose](introduction_mongoose.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
-  </si>
-  <si>
-    <t>[Mongoose - la suite](mongoose2.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 7 - Mongoose](exercice7_mongoose.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 8 - Express et JWT](exercice8_express_jwt.md)</t>
-  </si>
-  <si>
-    <t>Retour sur formatif &lt;br/&gt; [Express et JWT](express_jwt.md)</t>
-  </si>
-  <si>
-    <t>[Introduction à React](introduction_react.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 9 - React](exercice9_react.md)</t>
-  </si>
-  <si>
-    <t>[React et les styles](react_styles.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 10 - React et styles](exercice10_react_styles.md)</t>
-  </si>
-  <si>
-    <t>[Routes, contexte et API](react3.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 11 - Contexte et API](exercice11_context.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 12 - Internatialisation](exercice12_internationalisation.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 15 - Netlify](exercice15_netlify.md)</t>
-  </si>
-  <si>
-    <t>[Netlify](netlify.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 14 - PWA](exercice14_pwa.md)</t>
-  </si>
-  <si>
-    <t>[React et PWA](pwa.md)</t>
-  </si>
-  <si>
-    <t>[Authentification](authentification.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 13 - Authentification](exercice13_authentification.md)</t>
-  </si>
-  <si>
-    <t>[Internationalisation](internationalisation.md) &lt;br /&gt;[Accessibilité](accessibilite.md)</t>
+    <t>[Introduction à TypeScript](typescript/introduction_typescript.md)</t>
+  </si>
+  <si>
+    <t>[TypeScript 2](typescript/typescript_2.md)</t>
+  </si>
+  <si>
+    <t>[Introduction à React](react/introduction_react.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 9 - React](react/exercice9_react.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 10 - React et styles](react/exercice10_react_styles.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 11 - Contexte et API](react/exercice11_context.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 12 - Internatialisation](react/exercice12_internationalisation.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 13 - Authentification](react/exercice13_authentification.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 14 - PWA](react/exercice14_pwa.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 15 - Netlify](react/exercice15_netlify.md)</t>
+  </si>
+  <si>
+    <t>[React et les styles](react/react_styles.md)</t>
+  </si>
+  <si>
+    <t>[Routes, contexte et API](react/react3.md)</t>
+  </si>
+  <si>
+    <t>[Internationalisation](react/internationalisation.md) &lt;br /&gt;[Accessibilité](react/accessibilite.md)</t>
+  </si>
+  <si>
+    <t>[Authentification](react/authentification.md)</t>
+  </si>
+  <si>
+    <t>[React et PWA](react/pwa.md)</t>
+  </si>
+  <si>
+    <t>[Netlify](react/netlify.md)</t>
+  </si>
+  <si>
+    <t>[JavaScript asynchrone](typescript/javascript_async.md)</t>
   </si>
 </sst>
 </file>
@@ -624,13 +570,13 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -655,11 +601,9 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -669,10 +613,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -683,10 +624,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -697,10 +635,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,10 +649,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,10 +663,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -739,10 +677,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +691,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -764,10 +705,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -778,7 +719,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,9 +732,6 @@
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -799,9 +740,6 @@
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -810,9 +748,6 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -821,9 +756,6 @@
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -832,194 +764,125 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout règles de react au contenu du cours
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C58D26-ED15-4144-8F28-A93767E0951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4478E9E5-BC8D-0443-878F-2093E30BB905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1580" windowWidth="10000" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
+    <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
   <sheets>
     <sheet name="horaire" sheetId="1" r:id="rId1"/>
@@ -80,15 +80,9 @@
     <t>Retour sur formatif &lt;br/&gt; [Express et JWT](express_jwt.md)</t>
   </si>
   <si>
-    <t>[Introduction à React](introduction_react.md)</t>
-  </si>
-  <si>
     <t>[React et les styles](react_styles.md)</t>
   </si>
   <si>
-    <t>[Routes, contexte et API](react3.md)</t>
-  </si>
-  <si>
     <t>[Netlify](netlify.md)</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>[Exercice 14 - Netlify](exercice14_netlify.md)</t>
+  </si>
+  <si>
+    <t>[Routes, contexte et API](react3.md)&lt;br/&gt; [Régles de React](regles_react.md)</t>
+  </si>
+  <si>
+    <t>[Introduction à React](introduction_react.md)&lt;br/&gt; [Penser en React](penser_en_react.md)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,10 +542,10 @@
         <v>45525.635416666664</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,10 +556,10 @@
         <v>45527.34375</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,10 +570,10 @@
         <v>45532.635416666664</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,10 +706,10 @@
         <v>45574.635416666664</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,10 +720,10 @@
         <v>45576.34375</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,10 +734,10 @@
         <v>45588.635416666664</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,10 +748,10 @@
         <v>45590.34375</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -762,10 +762,10 @@
         <v>45595.635416666664</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,10 +776,10 @@
         <v>45597.34375</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -790,10 +790,10 @@
         <v>45604.635416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ajout section tests + dictionnaire anglais pour termes
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4478E9E5-BC8D-0443-878F-2093E30BB905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE864EE-4451-B14F-AB5D-0104E3C209B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
   <sheets>
     <sheet name="horaire" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,12 +101,6 @@
     <t>[TypeScript 2](typescript_2.md)&lt;br/&gt;[Express - Générateur](generateur_express.md)</t>
   </si>
   <si>
-    <t>[Intergiciels](intergiciels_express.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 3 - Intergiciels Express](exercice3_intergiciels_express.md)</t>
-  </si>
-  <si>
     <t>[Exercice 1 - lodash](exercice1_lodash.md)</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>[Introduction à React](introduction_react.md)&lt;br/&gt; [Penser en React](penser_en_react.md)</t>
+  </si>
+  <si>
+    <t>[Intergiciels](intergiciels_express.md)&lt;br/&gt;[Tester API](tester_api.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 3 - Intergiciels Express et Tests API](exercice3_intergiciels_express.md)</t>
   </si>
 </sst>
 </file>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +545,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -559,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,10 +570,10 @@
         <v>45532.635416666664</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,10 +706,10 @@
         <v>45574.635416666664</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,10 +734,10 @@
         <v>45588.635416666664</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ajout page de simulacre mongoose
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE864EE-4451-B14F-AB5D-0104E3C209B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78904E56-A2C1-D046-B176-012595C92B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
   </si>
   <si>
-    <t>[Mongoose - la suite](mongoose2.md)</t>
-  </si>
-  <si>
     <t>Retour sur formatif &lt;br/&gt; [Express et JWT](express_jwt.md)</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>[Exercice 3 - Intergiciels Express et Tests API](exercice3_intergiciels_express.md)</t>
+  </si>
+  <si>
+    <t>[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose](simulacre_mongoose.md)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,10 +542,10 @@
         <v>45525.635416666664</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,10 +556,10 @@
         <v>45527.34375</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,10 +570,10 @@
         <v>45532.635416666664</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
         <v>45546.635416666664</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -637,10 +637,10 @@
         <v>45553.635416666664</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,10 +706,10 @@
         <v>45574.635416666664</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,10 +720,10 @@
         <v>45576.34375</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,10 +734,10 @@
         <v>45588.635416666664</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,10 +748,10 @@
         <v>45590.34375</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -762,10 +762,10 @@
         <v>45595.635416666664</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,10 +776,10 @@
         <v>45597.34375</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -790,10 +790,10 @@
         <v>45604.635416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mise à jour section firebase
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D286B01-DCA3-1B44-9BE3-408BD22C3BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D91D7D-AE5E-B048-8B11-BBAA51E249D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -68,12 +68,6 @@
     <t>[JavaScript asynchrone](javascript_async.md) &lt;br/&gt; [MongoDB](mongodb.md)</t>
   </si>
   <si>
-    <t>[Netlify](netlify.md)</t>
-  </si>
-  <si>
-    <t>[React et PWA](pwa.md)</t>
-  </si>
-  <si>
     <t>[Authentification](authentification.md)</t>
   </si>
   <si>
@@ -113,12 +107,6 @@
     <t>[Exercice 12 - Authentification](exercice12_authentification.md)</t>
   </si>
   <si>
-    <t>[Exercice 13 - PWA](exercice13_pwa.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 14 - Netlify](exercice14_netlify.md)</t>
-  </si>
-  <si>
     <t>[Routes, contexte et API](react3.md)&lt;br/&gt; [Régles de React](regles_react.md)</t>
   </si>
   <si>
@@ -147,6 +135,15 @@
   </si>
   <si>
     <t>Retour sur formatif &lt;br/&gt; Projet API</t>
+  </si>
+  <si>
+    <t>[React et PWA](pwa.md)&lt;br/&gt;[Netlify](netlify.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 13 - PWA](exercice13_pwa.md)&lt;br/&gt;[Exercice 14 - Netlify](exercice14_netlify.md)</t>
+  </si>
+  <si>
+    <t>Formatif React</t>
   </si>
 </sst>
 </file>
@@ -511,7 +508,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,10 +539,10 @@
         <v>45525.635416666664</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,10 +553,10 @@
         <v>45527.34375</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,10 +567,10 @@
         <v>45532.635416666664</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,7 +584,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -598,10 +595,10 @@
         <v>45541.34375</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -612,10 +609,10 @@
         <v>45546.635416666664</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -637,7 +634,7 @@
         <v>45553.635416666664</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,10 +645,10 @@
         <v>45555.34375</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,10 +703,10 @@
         <v>45574.635416666664</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,10 +717,10 @@
         <v>45576.34375</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,10 +731,10 @@
         <v>45588.635416666664</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,10 +745,10 @@
         <v>45590.34375</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -762,10 +759,10 @@
         <v>45595.635416666664</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,10 +773,10 @@
         <v>45597.34375</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -790,10 +787,7 @@
         <v>45604.635416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -804,7 +798,7 @@
         <v>45609.635416666664</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -815,7 +809,7 @@
         <v>45611.34375</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remplacer exemple api par hotel25
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE64557-4DBB-4B42-8DA6-62B121ED053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EEF187-AA1F-D548-B028-0DC4D60143F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -162,15 +162,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,10 +191,29 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -191,9 +222,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +544,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45890.427083333336</v>
+        <v>45890.552083333336</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -552,8 +585,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>45894.59375</v>
+      <c r="B3" s="2">
+        <v>45894.510416666664</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -567,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>45897.427083333336</v>
+        <v>45897.552083333336</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -580,8 +613,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>45904.59375</v>
+      <c r="B5" s="2">
+        <v>45904.510416666664</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -595,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>45908.59375</v>
+        <v>45908.510416666664</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
@@ -608,8 +641,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>45911.427083333336</v>
+      <c r="B7" s="2">
+        <v>45911.552083333336</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -623,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>45915.59375</v>
+        <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -633,8 +666,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>45918.427083333336</v>
+      <c r="B9" s="2">
+        <v>45918.552083333336</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -645,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>45922.59375</v>
+        <v>45922.510416666664</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -658,8 +691,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>45925.427083333336</v>
+      <c r="B11" s="2">
+        <v>45925.552083333336</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -670,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>45929.59375</v>
+        <v>45929.510416666664</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -680,8 +713,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>45932.427083333336</v>
+      <c r="B13" s="2">
+        <v>45932.552083333336</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -692,7 +725,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>45936.59375</v>
+        <v>45936.510416666664</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -702,8 +735,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
-        <v>45939.427083333336</v>
+      <c r="B15" s="2">
+        <v>45939.552083333336</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -717,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>45950.59375</v>
+        <v>45950.510416666664</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -730,8 +763,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
-        <v>45953.427083333336</v>
+      <c r="B17" s="2">
+        <v>45953.552083333336</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -745,7 +778,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>45957.59375</v>
+        <v>45957.510416666664</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -758,8 +791,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
-        <v>45960.427083333336</v>
+      <c r="B19" s="2">
+        <v>45960.552083333336</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -773,7 +806,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>45967.427083333336</v>
+        <v>45967.552083333336</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -786,8 +819,8 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
-        <v>45971.59375</v>
+      <c r="B21" s="2">
+        <v>45971.510416666664</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -798,7 +831,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>45974.427083333336</v>
+        <v>45974.552083333336</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -808,8 +841,8 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
-        <v>45978.59375</v>
+      <c r="B23" s="2">
+        <v>45978.510416666664</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -820,7 +853,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>45981.427083333336</v>
+        <v>45981.552083333336</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -830,8 +863,8 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
-        <v>45985.59375</v>
+      <c r="B25" s="2">
+        <v>45985.510416666664</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -842,7 +875,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>45988.427083333336</v>
+        <v>45988.552083333336</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -852,8 +885,8 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
-        <v>45992.59375</v>
+      <c r="B27" s="2">
+        <v>45992.510416666664</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -864,7 +897,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>45995.427083333336</v>
+        <v>45995.552083333336</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -874,8 +907,8 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>45999.59375</v>
+      <c r="B29" s="2">
+        <v>45999.510416666664</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -886,7 +919,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>46002.427083333336</v>
+        <v>46002.552083333336</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -896,8 +929,8 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>46006.59375</v>
+      <c r="B31" s="3">
+        <v>46006.510416666664</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
modif mongoose + nouvel exemple
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C825E8-E691-914B-873E-C3689278BF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE53A49-0883-C14E-8FC4-D7810FE45547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -113,15 +113,9 @@
     <t>[Exercice 3 - Intergiciels Express et Tests API](exercice3_intergiciels_express.md)</t>
   </si>
   <si>
-    <t>[Mongoose](introduction_mongoose.md)&lt;br/&gt;[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose](simulacre_mongoose.md)</t>
-  </si>
-  <si>
     <t>Continuer les exercices</t>
   </si>
   <si>
-    <t>[Exercice 5 - Mongoose](exercice5_mongoose.md)&lt;br/&gt;[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
-  </si>
-  <si>
     <t>[React et les styles](react_styles.md)&lt;br/&gt; [TailWindCSS](react_tw.md)</t>
   </si>
   <si>
@@ -144,6 +138,18 @@
   </si>
   <si>
     <t xml:space="preserve">Retour sur formatif &lt;br/&gt; Projet API&lt;br/&gt;[Express et JWT](express_jwt.md) </t>
+  </si>
+  <si>
+    <t>[Mongoose](introduction_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose](simulacre_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 5 - Mongoose](exercice5_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +578,7 @@
         <v>45890.552083333336</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -586,7 +592,7 @@
         <v>45894.510416666664</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -600,7 +606,7 @@
         <v>45897.552083333336</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -639,10 +645,10 @@
         <v>45911.552083333336</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -653,10 +659,10 @@
         <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +684,7 @@
         <v>45922.510416666664</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -750,7 +756,7 @@
         <v>45950.510416666664</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -806,10 +812,10 @@
         <v>45967.552083333336</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -820,7 +826,7 @@
         <v>45971.510416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,7 +936,7 @@
         <v>46006.510416666664</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise a jour projet complet
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE53A49-0883-C14E-8FC4-D7810FE45547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B99ECF6-4412-674C-8F7A-EDF6AAAC389B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -143,13 +143,13 @@
     <t>[Mongoose](introduction_mongoose.md)</t>
   </si>
   <si>
-    <t>[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose](simulacre_mongoose.md)</t>
-  </si>
-  <si>
     <t>[Exercice 5 - Mongoose](exercice5_mongoose.md)</t>
   </si>
   <si>
     <t>[Exercice 6 - Mongoose](exercice6_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose dans un projet complet](projet_complet_mongoose.md)</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cours react 1 avec react 19
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B99ECF6-4412-674C-8F7A-EDF6AAAC389B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18004BCB-A604-1645-8C0E-F13733265C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>[Routes, contexte et API](react3.md)&lt;br/&gt; [Régles de React](regles_react.md)</t>
   </si>
   <si>
-    <t>[Introduction à React](introduction_react.md)&lt;br/&gt; [Penser en React](penser_en_react.md)</t>
-  </si>
-  <si>
     <t>[Intergiciels](intergiciels_express.md)&lt;br/&gt;[Tester API](tester_api.md)</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>[Mongoose - la suite](mongoose2.md)&lt;br/&gt;[Simulacre Mongoose dans un projet complet](projet_complet_mongoose.md)</t>
+  </si>
+  <si>
+    <t>[Introduction à React](introduction_react.md)&lt;br/&gt; [Structure typique d'un projet React](structure_projet_react.md)&lt;br/&gt; [Penser en React](penser_en_react.md)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>45890.552083333336</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -592,7 +592,7 @@
         <v>45894.510416666664</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -606,7 +606,7 @@
         <v>45897.552083333336</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,10 +617,10 @@
         <v>45904.510416666664</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -645,10 +645,10 @@
         <v>45911.552083333336</v>
       </c>
       <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
         <v>45922.510416666664</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -742,7 +742,7 @@
         <v>45939.552083333336</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -756,7 +756,7 @@
         <v>45950.510416666664</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -812,10 +812,10 @@
         <v>45967.552083333336</v>
       </c>
       <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
         <v>28</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>45971.510416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,7 +936,7 @@
         <v>46006.510416666664</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
react 19 et styles
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18004BCB-A604-1645-8C0E-F13733265C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BF8E0-2E4F-2F48-ACCA-A9D2E42F456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Continuer les exercices</t>
   </si>
   <si>
-    <t>[React et les styles](react_styles.md)&lt;br/&gt; [TailWindCSS](react_tw.md)</t>
-  </si>
-  <si>
     <t>Formatif React</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>[Introduction à React](introduction_react.md)&lt;br/&gt; [Structure typique d'un projet React](structure_projet_react.md)&lt;br/&gt; [Penser en React](penser_en_react.md)</t>
+  </si>
+  <si>
+    <t>[Styles : React et MUI](react_mui.md)&lt;br/&gt; [Styles : TailWindCSS](react_tw.md)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>45890.552083333336</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -592,7 +592,7 @@
         <v>45894.510416666664</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -645,10 +645,10 @@
         <v>45911.552083333336</v>
       </c>
       <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
         <v>45922.510416666664</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -742,7 +742,7 @@
         <v>45939.552083333336</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -756,7 +756,7 @@
         <v>45950.510416666664</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -812,10 +812,10 @@
         <v>45967.552083333336</v>
       </c>
       <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
         <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>45971.510416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,7 +936,7 @@
         <v>46006.510416666664</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
séparer cours route et contexte
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BF8E0-2E4F-2F48-ACCA-A9D2E42F456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205FCF83-A84C-304F-A87B-D0471D25B5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="25920" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>[Authentification](authentification.md)</t>
   </si>
   <si>
-    <t>[Internationalisation](internationalisation.md) &lt;br /&gt;[Accessibilité](accessibilite.md)</t>
-  </si>
-  <si>
     <t>[Exercice 1 - lodash](exercice1_lodash.md)</t>
   </si>
   <si>
@@ -92,15 +89,6 @@
     <t>[Exercice 9 - React et styles](exercice9_react_styles.md)</t>
   </si>
   <si>
-    <t>[Exercice 10 - Contexte et API](exercice10_context.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 11 - Internatialisation](exercice11_internationalisation.md)</t>
-  </si>
-  <si>
-    <t>[Exercice 12 - Authentification](exercice12_authentification.md)</t>
-  </si>
-  <si>
     <t>[Routes, contexte et API](react3.md)&lt;br/&gt; [Régles de React](regles_react.md)</t>
   </si>
   <si>
@@ -150,6 +138,18 @@
   </si>
   <si>
     <t>[Styles : React et MUI](react_mui.md)&lt;br/&gt; [Styles : TailWindCSS](react_tw.md)</t>
+  </si>
+  <si>
+    <t>[Contexte et API](react4.md)&lt;br/&gt; [Régles de React](regles_react.md)&lt;br/&gt; [Internationalisation](internationalisation.md) &lt;br /&gt;[Accessibilité](accessibilite.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 11 - Contexte et API](exercice11_context.md)&lt;br/&gt;[Exercice 12 - Internatialisation](exercice12_internationalisation.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 13 - Authentification](exercice13_authentification.md)</t>
+  </si>
+  <si>
+    <t>[Exercice 10 - Routes](exercice10_routes.md)</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,10 +578,10 @@
         <v>45890.552083333336</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -592,10 +592,10 @@
         <v>45894.510416666664</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -606,7 +606,7 @@
         <v>45897.552083333336</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,10 +617,10 @@
         <v>45904.510416666664</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -645,10 +645,10 @@
         <v>45911.552083333336</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>45915.510416666664</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,10 +684,10 @@
         <v>45922.510416666664</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -742,10 +742,10 @@
         <v>45939.552083333336</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -756,10 +756,10 @@
         <v>45950.510416666664</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -770,10 +770,10 @@
         <v>45953.552083333336</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -784,10 +784,10 @@
         <v>45957.510416666664</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -801,7 +801,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -812,10 +812,10 @@
         <v>45967.552083333336</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>45971.510416666664</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,7 +936,7 @@
         <v>46006.510416666664</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>